<commit_message>
Suma de puntos COSMIC
</commit_message>
<xml_diff>
--- a/AdministracionCOSMIC.xlsx
+++ b/AdministracionCOSMIC.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DARKENSES\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\Documents\GitHub\QuarterToPill\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Edatos" sheetId="1" r:id="rId1"/>
     <sheet name="Resultados" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="29">
   <si>
     <t>Proceso Funcional</t>
   </si>
@@ -60,24 +60,12 @@
     <t>Crear pill</t>
   </si>
   <si>
-    <t>Notificaciones</t>
-  </si>
-  <si>
     <t>Editar pill</t>
   </si>
   <si>
     <t>Notificar</t>
   </si>
   <si>
-    <t>Guardar Información</t>
-  </si>
-  <si>
-    <t>Leer Registro</t>
-  </si>
-  <si>
-    <t>Leer Información</t>
-  </si>
-  <si>
     <t>Entradas (E)</t>
   </si>
   <si>
@@ -102,13 +90,34 @@
     <t>Pts CÓSMICOS!</t>
   </si>
   <si>
-    <t>Guardar Registro</t>
+    <t>Lectura  Registro</t>
+  </si>
+  <si>
+    <t>Escritura Registro</t>
+  </si>
+  <si>
+    <t>Entrada Información</t>
+  </si>
+  <si>
+    <t>Salida Información</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Notificar tomar píldora</t>
+  </si>
+  <si>
+    <t>Pts COSMIC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -289,6 +298,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -298,7 +315,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -308,13 +324,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,86 +656,84 @@
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
     </row>
     <row r="2" spans="1:21" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="17"/>
+      <c r="B2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="25"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="23" t="s">
-        <v>21</v>
+      <c r="I3" s="16"/>
+      <c r="J3" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="23"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="17"/>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="23"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="17"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -738,21 +745,31 @@
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="10"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="10"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
     </row>
@@ -760,29 +777,39 @@
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="10"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="P5" s="10"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="U5" s="10"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -792,21 +819,31 @@
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="23"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="10"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
     </row>
@@ -817,20 +854,28 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="23"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="23"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
@@ -842,46 +887,52 @@
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="23"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="23"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="23"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
     </row>
-    <row r="9" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
+    <row r="9" spans="1:21" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -890,20 +941,30 @@
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="10"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="L10" s="10"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="10"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="P10" s="10"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="23"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="17"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
@@ -915,70 +976,100 @@
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="10"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="P11" s="10"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="23"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="23"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="23"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="10"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="S12" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="23"/>
+        <v>27</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="17"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="23"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="23"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="17"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
       <c r="U13" s="10"/>
@@ -1000,56 +1091,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-      <c r="G1" s="19" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="G1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="21"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:11" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <f>COUNTIF(Edatos!B3:U3,"E")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="5">
         <f>COUNTIF(Edatos!C3:V3,"X")</f>
@@ -1080,11 +1171,11 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <f>COUNTIF(Edatos!B4:U4,"E")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5">
         <f>COUNTIF(Edatos!C4:V4,"X")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5">
         <f>COUNTIF(Edatos!D4:W4,"R")</f>
@@ -1092,7 +1183,7 @@
       </c>
       <c r="D4" s="5">
         <f>COUNTIF(Edatos!E4:X4,"W")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5">
         <v>1</v>
@@ -1110,19 +1201,19 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <f>COUNTIF(Edatos!B5:U5,"E")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" s="5">
         <f>COUNTIF(Edatos!C5:V5,"X")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="5">
         <f>COUNTIF(Edatos!D5:W5,"R")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5">
         <f>COUNTIF(Edatos!E5:X5,"W")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="5">
         <v>1</v>
@@ -1140,19 +1231,19 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <f>COUNTIF(Edatos!B6:U6,"E")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="5">
         <f>COUNTIF(Edatos!C6:V6,"X")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="5">
         <f>COUNTIF(Edatos!D6:W6,"R")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5">
         <f>COUNTIF(Edatos!E6:X6,"W")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -1170,19 +1261,19 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <f>COUNTIF(Edatos!B7:U7,"E")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="5">
         <f>COUNTIF(Edatos!C7:V7,"X")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="5">
         <f>COUNTIF(Edatos!D7:W7,"R")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5">
         <f>COUNTIF(Edatos!E7:X7,"W")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="5">
         <v>1</v>
@@ -1200,15 +1291,15 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <f>COUNTIF(Edatos!B8:U8,"E")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" s="5">
         <f>COUNTIF(Edatos!C8:V8,"X")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="5">
         <f>COUNTIF(Edatos!D8:W8,"R")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5">
         <f>COUNTIF(Edatos!E8:X8,"W")</f>
@@ -1260,7 +1351,7 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <f>COUNTIF(Edatos!B10:U10,"E")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" s="5">
         <f>COUNTIF(Edatos!C10:V10,"X")</f>
@@ -1268,11 +1359,11 @@
       </c>
       <c r="C10" s="5">
         <f>COUNTIF(Edatos!D10:W10,"R")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10" s="5">
         <f>COUNTIF(Edatos!E10:X10,"W")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="5">
         <v>1</v>
@@ -1290,11 +1381,11 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <f>COUNTIF(Edatos!B11:U11,"E")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" s="5">
         <f>COUNTIF(Edatos!C11:V11,"X")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11" s="5">
         <f>COUNTIF(Edatos!D11:W11,"R")</f>
@@ -1302,7 +1393,7 @@
       </c>
       <c r="D11" s="5">
         <f>COUNTIF(Edatos!E11:X11,"W")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="5">
         <v>1</v>
@@ -1320,19 +1411,19 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <f>COUNTIF(Edatos!B12:U12,"E")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B12" s="5">
         <f>COUNTIF(Edatos!C12:V12,"X")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="5">
         <f>COUNTIF(Edatos!D12:W12,"R")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="5">
         <f>COUNTIF(Edatos!E12:X12,"W")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
@@ -1350,11 +1441,11 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <f>COUNTIF(Edatos!B13:U13,"E")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B13" s="5">
         <f>COUNTIF(Edatos!C13:V13,"X")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="5">
         <f>COUNTIF(Edatos!D13:W13,"R")</f>
@@ -1362,10 +1453,10 @@
       </c>
       <c r="D13" s="5">
         <f>COUNTIF(Edatos!E13:X13,"W")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G13" s="7">
         <v>0</v>
@@ -1380,29 +1471,29 @@
         <v>0</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f>SUM(A3:A13)</f>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2">
         <f>SUM(B3:B13)</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2">
         <f>SUM(C3:C13)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D14" s="2">
         <f>SUM(D3:D13)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E14" s="13">
         <f>SUM(A14:D14)</f>
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="G14" s="2">
         <f>SUM(G3:G13)</f>

</xml_diff>